<commit_message>
update layout to 6up with larger mousebites
</commit_message>
<xml_diff>
--- a/pcb/led_jewellery/led_jewellery-bom.xlsx
+++ b/pcb/led_jewellery/led_jewellery-bom.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">100R</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R2</t>
+    <t xml:space="preserve">R1,R2,R3,R4,R5,R6</t>
   </si>
   <si>
     <t xml:space="preserve">R_0805_2012Metric</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">SW_SPST</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1,SW2</t>
+    <t xml:space="preserve">SW1,SW2,SW3,SW4,SW5,SW6</t>
   </si>
   <si>
     <t xml:space="preserve">diptronics_ta3</t>
@@ -266,7 +266,7 @@
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.41"/>
   </cols>

</xml_diff>